<commit_message>
Estimate the effect of female bargaining power
Here first I estimated the determinants of the female bargaining indices, comparing them to commonly used variables as proxy for bargaining power. Then I use the index as explanatory variables in the children outcomes regression. I implemented a fixed effects model.
</commit_message>
<xml_diff>
--- a/Outputs/dec.csv.xlsx
+++ b/Outputs/dec.csv.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/500a1adc9097afdd/Desktop/Development Economics MSc/Dissertation/R/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{B5D7743D-BD56-4D07-B028-3D91DE7057CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6D263F15-EF5D-4D5C-A218-3C3F873B122B}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{B5D7743D-BD56-4D07-B028-3D91DE7057CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{175605D8-D5BD-47D2-9035-C62A8FB5E596}"/>
   <bookViews>
-    <workbookView xWindow="36285" yWindow="3540" windowWidth="17280" windowHeight="8970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13176" yWindow="4212" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="dec" sheetId="1" r:id="rId1"/>
-    <sheet name="table_pca" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
+    <sheet name="table pca sep" sheetId="5" r:id="rId1"/>
+    <sheet name="dec" sheetId="1" r:id="rId2"/>
+    <sheet name="table_pca" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>decision_mom</t>
   </si>
@@ -163,6 +164,27 @@
   </si>
   <si>
     <t>Correlation 2</t>
+  </si>
+  <si>
+    <t>Index type</t>
+  </si>
+  <si>
+    <t>Financial</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Loadings</t>
+  </si>
+  <si>
+    <t>Source: MxFLS-1, MxFLS-2 and MxFLS-3.</t>
   </si>
 </sst>
 </file>
@@ -172,9 +194,9 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,6 +383,13 @@
       <name val="LM Sans 12"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="LM Sans 12"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -543,7 +572,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -798,6 +827,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -844,7 +882,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -904,6 +942,30 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -922,23 +984,10 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="23" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="21" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1295,6 +1344,230 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E492207A-8A11-4671-AB86-802CC9924149}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="5" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="26">
+        <v>0.53970545677688897</v>
+      </c>
+      <c r="D2" s="27">
+        <v>1.37667392359985</v>
+      </c>
+      <c r="E2" s="27">
+        <v>0.74299842876929101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="26">
+        <v>0.50398889028827099</v>
+      </c>
+      <c r="D3" s="27">
+        <v>1.0592137788740099</v>
+      </c>
+      <c r="E3" s="27">
+        <v>0.53383197699275697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="26">
+        <v>0.42341543795804898</v>
+      </c>
+      <c r="D4" s="27">
+        <v>0.92052250214442299</v>
+      </c>
+      <c r="E4" s="27">
+        <v>0.38976343839571997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="27">
+        <v>0.39567673061710801</v>
+      </c>
+      <c r="D5" s="27">
+        <v>0.83535105532715603</v>
+      </c>
+      <c r="E5" s="27">
+        <v>0.3305289744894</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="27">
+        <v>0.34477892937097498</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0.66156028911442299</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0.228092048195224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="26">
+        <v>0.55332079118451705</v>
+      </c>
+      <c r="D7" s="27">
+        <v>1.59832438920402</v>
+      </c>
+      <c r="E7" s="27">
+        <v>0.88438611560388003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="26">
+        <v>0.54275406640208701</v>
+      </c>
+      <c r="D8" s="27">
+        <v>0.992106200944043</v>
+      </c>
+      <c r="E8" s="27">
+        <v>0.538469674865106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0.49158174604520999</v>
+      </c>
+      <c r="D9" s="27">
+        <v>0.87223896806004597</v>
+      </c>
+      <c r="E9" s="27">
+        <v>0.42877675488763001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="27">
+        <v>0.35855786994736499</v>
+      </c>
+      <c r="D10" s="27">
+        <v>0.70170192328326497</v>
+      </c>
+      <c r="E10" s="27">
+        <v>0.25160074695041601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="27">
+        <v>0.17040471325902501</v>
+      </c>
+      <c r="D11" s="27">
+        <v>0.45595836035938297</v>
+      </c>
+      <c r="E11" s="27">
+        <v>7.7697453655095894E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.4">
+      <c r="A12" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
@@ -1864,11 +2137,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B955D1-0265-40AD-9554-CD3B98403D6E}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1885,7 +2158,7 @@
       <c r="B1" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="24" t="s">
         <v>39</v>
       </c>
       <c r="D1" s="20" t="s">
@@ -1902,19 +2175,19 @@
       <c r="A2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="26">
         <v>0.50406715844816496</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="27">
         <v>3.60096795540676E-2</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="27">
         <v>1.6414921329435099</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="27">
         <v>0.82742227506785404</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="27">
         <v>5.9109605697818798E-2</v>
       </c>
     </row>
@@ -1922,19 +2195,19 @@
       <c r="A3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="26">
         <v>0.49021415678302899</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="27">
         <v>4.1201267258123703E-2</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="27">
         <v>1.35478759319496</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="27">
         <v>0.66413605761817496</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="27">
         <v>5.5818965705215599E-2</v>
       </c>
     </row>
@@ -1942,19 +2215,19 @@
       <c r="A4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="26">
         <v>0.46156936074353999</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="27">
         <v>-0.14446131456465799</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="27">
         <v>1.1852249183746999</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="27">
         <v>0.54706350791152303</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="27">
         <v>-0.17121914976319799</v>
       </c>
     </row>
@@ -1962,19 +2235,19 @@
       <c r="A5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="26">
         <v>0.32682068961019101</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="27">
         <v>0.14492466958810701</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="27">
         <v>1.0158179447606499</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="27">
         <v>0.33199032122508099</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="27">
         <v>0.147217080006106</v>
       </c>
     </row>
@@ -1982,19 +2255,19 @@
       <c r="A6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="27">
         <v>0.22728666794032601</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="26">
         <v>-0.45015079752863901</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="27">
         <v>0.95537229708341098</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="27">
         <v>0.21714338604658301</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="27">
         <v>-0.43006160146886502</v>
       </c>
     </row>
@@ -2002,19 +2275,19 @@
       <c r="A7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="27">
         <v>0.22216709069884399</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="26">
         <v>0.28315662976737199</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="27">
         <v>0.917928364482408</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="27">
         <v>0.203933474207005</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="27">
         <v>0.25991750205471498</v>
       </c>
     </row>
@@ -2022,19 +2295,19 @@
       <c r="A8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="27">
         <v>0.186041055950072</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="26">
         <v>0.31693819219546299</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="27">
         <v>0.85985901944127996</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="27">
         <v>0.159969079945049</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="27">
         <v>0.27252216316468297</v>
       </c>
     </row>
@@ -2042,19 +2315,19 @@
       <c r="A9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="27">
         <v>0.16252599858018099</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="27">
         <v>-8.4900704051837195E-2</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="27">
         <v>0.80874497955301605</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="27">
         <v>0.131442085398562</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="27">
         <v>-6.8663018162439707E-2</v>
       </c>
     </row>
@@ -2062,19 +2335,19 @@
       <c r="A10" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="27">
         <v>0.144145650414501</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="27">
         <v>-0.18209741733072499</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="27">
         <v>0.78012947134105404</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="27">
         <v>0.112452270053977</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="27">
         <v>-0.14205956191478999</v>
       </c>
     </row>
@@ -2082,19 +2355,19 @@
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="27">
         <v>2.8630952780076699E-2</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="26">
         <v>0.38699714632466198</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="27">
         <v>0.72722872815293504</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="27">
         <v>2.0821251376061899E-2</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="27">
         <v>0.28143544252049901</v>
       </c>
     </row>
@@ -2102,39 +2375,39 @@
       <c r="A12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="27">
         <v>1.0941500460825501E-2</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="26">
         <v>0.514448265517647</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="27">
         <v>0.69473820033102895</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="27">
         <v>7.6014783390750502E-3</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="27">
         <v>0.35740686214914902</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.45">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="28">
         <v>-4.4581448828620501E-2</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="29">
         <v>0.34216791787101702</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="28">
         <v>0.51432527164067898</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="28">
         <v>-2.29293657789153E-2</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="28">
         <v>0.17598560730573601</v>
       </c>
     </row>
@@ -2144,7 +2417,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
@@ -2160,28 +2433,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="26">
+      <c r="C1" s="34">
         <v>2002</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="26">
+      <c r="D1" s="35"/>
+      <c r="E1" s="34">
         <v>2005</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="26">
+      <c r="F1" s="35"/>
+      <c r="G1" s="34">
         <v>2009</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:11" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="25"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="10" t="s">
         <v>21</v>
       </c>
@@ -2532,7 +2805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Attrition and shift shares
Here I implemented robustness checks proofs which included the construction of the Bartik-like instruments to do a new regression design. I will include this on the main results.
</commit_message>
<xml_diff>
--- a/Outputs/dec.csv.xlsx
+++ b/Outputs/dec.csv.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/500a1adc9097afdd/Desktop/Development Economics MSc/Dissertation/R/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{B5D7743D-BD56-4D07-B028-3D91DE7057CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{175605D8-D5BD-47D2-9035-C62A8FB5E596}"/>
+  <xr:revisionPtr revIDLastSave="235" documentId="8_{B5D7743D-BD56-4D07-B028-3D91DE7057CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{14FD2B9C-166A-4743-A708-1CADFC9A94D3}"/>
   <bookViews>
-    <workbookView xWindow="13176" yWindow="4212" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table pca sep" sheetId="5" r:id="rId1"/>
     <sheet name="dec" sheetId="1" r:id="rId2"/>
     <sheet name="table_pca" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="84">
   <si>
     <t>decision_mom</t>
   </si>
@@ -185,6 +186,163 @@
   </si>
   <si>
     <t>Source: MxFLS-1, MxFLS-2 and MxFLS-3.</t>
+  </si>
+  <si>
+    <t>Mom makes more decisions</t>
+  </si>
+  <si>
+    <t>Dad makes more decisions</t>
+  </si>
+  <si>
+    <t>Attrited at some point (4)</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Attends school? (%)</t>
+  </si>
+  <si>
+    <t>Worked last 12 months? (%)</t>
+  </si>
+  <si>
+    <t>Mom works? (%)</t>
+  </si>
+  <si>
+    <t>Dad works? (%)</t>
+  </si>
+  <si>
+    <t>Mom household head (%)</t>
+  </si>
+  <si>
+    <t>Boys (%)</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Education level</t>
+  </si>
+  <si>
+    <t>Household per capita income</t>
+  </si>
+  <si>
+    <t>Number of children</t>
+  </si>
+  <si>
+    <t>Number of persons</t>
+  </si>
+  <si>
+    <t>Number of decisions mom</t>
+  </si>
+  <si>
+    <t>&lt;0.001***</t>
+  </si>
+  <si>
+    <t>0.001***</t>
+  </si>
+  <si>
+    <t>&gt;0.9</t>
+  </si>
+  <si>
+    <t>0.005***</t>
+  </si>
+  <si>
+    <t>0.008***</t>
+  </si>
+  <si>
+    <t>Present 3 waves        (2)</t>
+  </si>
+  <si>
+    <t>p-value       (3)</t>
+  </si>
+  <si>
+    <t>Present 3 waves         (5)</t>
+  </si>
+  <si>
+    <t>p-value       (6)</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="LM Sans 12"/>
+        <family val="3"/>
+      </rPr>
+      <t>Variables ending with (%) are dichotomous</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="LM Sans 12"/>
+        <family val="3"/>
+      </rPr>
+      <t>Two sample test for equality of proportions; Welch Two Sample t-test</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="LM Sans 12"/>
+        <family val="3"/>
+      </rPr>
+      <t>*p&lt;0.1; **p&lt;0.05; ***p&lt;0.01</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="LM Sans 12"/>
+        <family val="3"/>
+      </rPr>
+      <t>Education level is classified into ten categories. 1. No education, 2. Preschool, 3. Elementary, 4. Secondary, 5. Open secondary, 6. High school, 7. Open high school, 8. Normal Basic, 9. College, and 10. Graduate</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="LM Sans 12"/>
+        <family val="3"/>
+      </rPr>
+      <t>(%); Mean</t>
+    </r>
+  </si>
+  <si>
+    <t>0.012**</t>
+  </si>
+  <si>
+    <t>Raven z-score</t>
+  </si>
+  <si>
+    <t>Height z-score</t>
+  </si>
+  <si>
+    <t>Attrited at some point (1)</t>
   </si>
 </sst>
 </file>
@@ -196,7 +354,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,8 +548,28 @@
       <name val="LM Sans 12"/>
       <family val="3"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="LM Sans 12"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="LM Sans 12"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="LM Sans 12"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,8 +749,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -836,6 +1020,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -882,7 +1118,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -962,32 +1198,84 @@
     </xf>
     <xf numFmtId="165" fontId="21" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1347,7 +1635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E492207A-8A11-4671-AB86-802CC9924149}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
@@ -1546,20 +1834,20 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.4">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2142,7 +2430,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A5" sqref="A5:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2421,7 +2709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
@@ -2433,28 +2721,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="34">
+      <c r="C1" s="37">
         <v>2002</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="34">
+      <c r="D1" s="38"/>
+      <c r="E1" s="37">
         <v>2005</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="34">
+      <c r="F1" s="38"/>
+      <c r="G1" s="37">
         <v>2009</v>
       </c>
-      <c r="H1" s="36"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:11" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="33"/>
-      <c r="B2" s="31"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="10" t="s">
         <v>21</v>
       </c>
@@ -2806,6 +3094,463 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66C1532-09A9-40F5-8F21-7ACC0A3C501E}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
+    <col min="5" max="6" width="12.21875" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A1" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="53"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+    </row>
+    <row r="2" spans="1:7" ht="52.2" x14ac:dyDescent="0.45">
+      <c r="A2" s="42"/>
+      <c r="B2" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A3" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="55">
+        <v>0.95</v>
+      </c>
+      <c r="C3" s="55">
+        <v>0.94</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="55">
+        <v>0.95</v>
+      </c>
+      <c r="F3" s="55">
+        <v>0.94</v>
+      </c>
+      <c r="G3" s="43">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A4" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="56">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C4" s="56">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="56">
+        <v>0.02</v>
+      </c>
+      <c r="F4" s="56">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A5" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="55">
+        <v>0.31</v>
+      </c>
+      <c r="C5" s="55">
+        <v>0.26</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="55">
+        <v>0.26</v>
+      </c>
+      <c r="F5" s="55">
+        <v>0.22</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A6" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="55">
+        <v>0.97</v>
+      </c>
+      <c r="C6" s="55">
+        <v>0.97</v>
+      </c>
+      <c r="D6" s="43">
+        <v>0.6</v>
+      </c>
+      <c r="E6" s="55">
+        <v>0.97</v>
+      </c>
+      <c r="F6" s="55">
+        <v>0.97</v>
+      </c>
+      <c r="G6" s="43">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A7" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="56">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="C7" s="56">
+        <v>5.5E-2</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="56">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F7" s="56">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A8" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="55">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="55">
+        <v>0.49</v>
+      </c>
+      <c r="D8" s="43">
+        <v>0.6</v>
+      </c>
+      <c r="E8" s="55">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="55">
+        <v>0.48</v>
+      </c>
+      <c r="G8" s="43">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A9" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="43">
+        <v>10.1</v>
+      </c>
+      <c r="C9" s="43">
+        <v>7.5</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="43">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="F9" s="43">
+        <v>7.2</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A10" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="43">
+        <v>3.31</v>
+      </c>
+      <c r="C10" s="43">
+        <v>3</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="43">
+        <v>3.25</v>
+      </c>
+      <c r="F10" s="43">
+        <v>2.94</v>
+      </c>
+      <c r="G10" s="43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A11" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="C11" s="43">
+        <v>-0.02</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="43">
+        <v>-0.03</v>
+      </c>
+      <c r="F11" s="43">
+        <v>-0.08</v>
+      </c>
+      <c r="G11" s="43">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A12" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="43">
+        <v>0.08</v>
+      </c>
+      <c r="C12" s="43">
+        <v>-0.03</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="43">
+        <v>-0.02</v>
+      </c>
+      <c r="F12" s="43">
+        <v>-0.12</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A13" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="57">
+        <v>12419</v>
+      </c>
+      <c r="C13" s="57">
+        <v>10858</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="57">
+        <v>11769</v>
+      </c>
+      <c r="F13" s="57">
+        <v>10269</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A14" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="43">
+        <v>3.5</v>
+      </c>
+      <c r="C14" s="43">
+        <v>3.51</v>
+      </c>
+      <c r="D14" s="43">
+        <v>0.8</v>
+      </c>
+      <c r="E14" s="43">
+        <v>3.55</v>
+      </c>
+      <c r="F14" s="43">
+        <v>3.54</v>
+      </c>
+      <c r="G14" s="43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A15" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="43">
+        <v>6</v>
+      </c>
+      <c r="C15" s="43">
+        <v>6</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="43">
+        <v>6</v>
+      </c>
+      <c r="F15" s="43">
+        <v>6</v>
+      </c>
+      <c r="G15" s="43">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A16" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="46">
+        <v>9.26</v>
+      </c>
+      <c r="C16" s="46">
+        <v>9.31</v>
+      </c>
+      <c r="D16" s="46">
+        <v>0.2</v>
+      </c>
+      <c r="E16" s="46">
+        <v>7.1</v>
+      </c>
+      <c r="F16" s="46">
+        <v>7.31</v>
+      </c>
+      <c r="G16" s="46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+    </row>
+    <row r="18" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+    </row>
+    <row r="19" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+    </row>
+    <row r="20" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+    </row>
+    <row r="21" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+    </row>
+    <row r="22" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>